<commit_message>
all manifesto items have been added
</commit_message>
<xml_diff>
--- a/data/2014_bjp_manifesto.xlsx
+++ b/data/2014_bjp_manifesto.xlsx
@@ -631,6 +631,10 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>India has always been a caring society. It is in our culture to help the aged, the weak and the helpless. We have to retain this. We have to educate our younger generations about this. The social security schemes of the Governments have to be made more meaningful. Our aspirations get frustrated when we encounter a weak social infrastructure. We need it on a daily basis.
+</t>
+  </si>
+  <si>
     <t>ChildrentheFutureoftheNation</t>
   </si>
   <si>
@@ -640,6 +644,22 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;blockquote&gt;"There can be no keener revelation of a society's soul than the way in which it treats its children"&lt;/blockquote&gt; - Nelson Mandela
+&lt;p&gt;Indicators related to children welfare are an indicator of the progress of the nation, be it health, education or safety of children. Under the UPA rule, the same has not been given its due weightage. BJP is committed to address the issues related to children, like malnutrition and under-nutrition, problem of child labour, child-trafficking and missing children, sexual abuse, school dropouts and the increasing crime rate among juveniles. BJP will take the following steps to ensure survival, development, participation and protection of children:
+&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Lay special emphasis on vulnerable children and especially those belonging to the vulnerable communities like SCs, STs, OBCs, migrants, slum dwellers, street dwellers and those with disabilities.&lt;/li&gt;
+ &lt;li&gt;Ensure effective implementation of the Right to Education, Right to Food Security Act.&lt;/li&gt;
+ &lt;li&gt;Review, amend and strengthen the Child and Adolescent Labour (Prohibition and Regulation) Act,
+ 2012 and Integrated Child Protection Scheme (ICPS).&lt;/li&gt;
+&lt;li&gt; Focused efforts will be made to address issue of anaemia.&lt;/li&gt;
+ &lt;li&gt;Reduce the burden of books on children without compromising on the quality of education.&lt;/li&gt;
+ &lt;li&gt;Endeavour to inculcate values amongst children.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>SeniorCitizens</t>
   </si>
   <si>
@@ -649,6 +669,18 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP is committed to the welfare of senior citizens, especially their security and health care. We will take measures to deal with the issues related to the senior citizens in a focused manner.
+BJP will:
+&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Provide financial support, exploring ideas like additional tax benefits and higher interest rates.&lt;/li&gt;
+ &lt;li&gt;Invest in setting up and improving old-age homes.&lt;/li&gt;
+ &lt;li&gt;Harness their experience in the National Interest. Devise schemes and programs to engage the senior citizens as volunteers / part time workers in various development programmes of the government, in urban and rural areas. This will not only help in utilizing their time, but also it would be an effective utilization of their experience and may add an additional source of income for them.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>SpeciallyAbled</t>
   </si>
   <si>
@@ -658,6 +690,23 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;About 70 million people are suffering from disability, and BJP considers it a serious neglect. The welfare and rehabilitation of disabled people is integral to our vision of a caring society and that of a responsive government. The BJP commits to:
+&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Enact the 'Rights of the Persons with Disabilities bill' (RPWD).&lt;/li&gt;
+ &lt;li&gt;Use technology to deliver low cost quality education to specially-abled students 'in-home' - through
+ E-learning.&lt;/li&gt;
+ &lt;li&gt;Identify each and every special needs person across the country - establishing a web based disability registration system to issue universal ID for all applicable government benefits (healthcare, transportation, jobs, education etc).&lt;/li&gt;
+ &lt;li&gt;Ensure disabled friendly access to public facilities, public buildings and transport.&lt;/li&gt;
+ &lt;li&gt;Ensure maximum economic independence of the disabled by creating more income generation
+ models for them.&lt;/li&gt;
+ &lt;li&gt;Support and aid voluntary organizations working for the care of the disabled.&lt;/li&gt;
+ &lt;li&gt;Provide a higher tax relief for the family member taking care of the disabled.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>YouthMakingIndiaUnstoppable</t>
   </si>
   <si>
@@ -667,6 +716,22 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;blockquote&gt;'Young men, my hope is in you. Will you respond to the call of your nation? Each one of you has a glorious future if you dare believe me. Have a tremendous faith in yourselves, like the faith I had when I was a child, and which I am working out now. Have that faith, each one of you, in yourself-that eternal power is lodged in every soul-and you will revive the whole of the country.'&lt;/blockquote&gt; - Swami Vivekananda
+&lt;p&gt;BJP considers youth as the most productive asset of the nation who have played a key role in taking the country to a near double digit growth. All sectors dominated by youth are doing exceptionally well. India is the oldest civilization but the youngest country and this necessitates that the policies must be based on the judicious mix of experience of energy, and be 'Youth inclusive', so that youth are an integral part of the development process. We commit to review and revise policies to seek participation of youth in decision-making and nation building process and actively get the youth to participate in decision-making bodies.
+&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;we will initiate the 'Young Leaders programme' in all sectors, to recognize, reward and involve these exceptionally talented youth to serve as role models and mentors for others.&lt;/li&gt;
+ &lt;li&gt;set up the National Youth Advisory Council.&lt;/li&gt;
+ &lt;li&gt;BJP will initiate nation-wide 'district level incubation and accelerator programme' for encouraging
+ innovation and entrepreneurship.&lt;/li&gt;
+ &lt;li&gt;procedure to avail Student's loans will be simplified and loans made affordable.&lt;/li&gt;
+ &lt;li&gt;set up neighbourhood Children's/ Youth Parliament across India that leads to vibrant student committees.&lt;/li&gt;
+ &lt;li&gt;Will launch a programme, 'Youth for Development'.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>PromotionofSports</t>
   </si>
   <si>
@@ -676,6 +741,23 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP recognizes the importance of sports in society and for all age groups. Sports have a direct relation to fitness, good health and productivity. India has not fared well in sports, and needs to invest for promotion of sports in an organized manner.&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;BJP will promote all sports - traditional and modern.&lt;/li&gt;
+ &lt;li&gt;More funds will be allocated to sports, and we will encourage the State Governments to fully
+ discharge their responsibility in the promotion of sports.&lt;/li&gt;
+ &lt;li&gt;Steps would be taken to inculcate a culture of sports at the school level by arranging sports facilities and training needs for promoting a healthy lifestyle, and making sports as a compulsory part of the school curriculum.&lt;/li&gt;
+ &lt;li&gt;Launch a 'National Sports Talent Search System', so that extraordinary sporting talent is identified at a very young age. Such promising boys and girls will be selected for special training. The existing rural sports programme and National Women Sports Festival will be broadened to reach every village and to identify talent for nurturing and excellence development.&lt;/li&gt;
+ &lt;li&gt;Attractive career path needs to be planned for sportspersons providing security of career through jobs in government, PSUs and private sector.&lt;/li&gt;
+ &lt;li&gt;Establish sports academies across the country.&lt;/li&gt;
+ &lt;li&gt;Special scheme would be devised for sportspersons to ensure social security.&lt;/li&gt;
+ &lt;li&gt;Encourage business houses to patronize sports and sportspersons.&lt;/li&gt;
+ &lt;li&gt;Mandate all new housing colonies to include sports facilities.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>WomenTheNationBuilder</t>
   </si>
   <si>
@@ -685,6 +767,36 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP recognizes the important role of women in development of the society and growth of the nation, and remains committed to give a high priority to Women's Empowerment and welfare. BJP ruled states have demonstrated this through various schemes. BJP also recognizes the need for women's security as a precondition to women's empowerment and will undertake the following for women welfare:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Women's welfare and development will be accorded a high priority at all levels within the government, and BJP is committed to 33% reservation in parliamentary and state assemblies through a constitutional amendment.&lt;/li&gt;
+ &lt;li&gt;Launch a national campaign for saving the girl child and educating her - Beti Bachao - Beti Padhao.&lt;/li&gt;
+ &lt;li&gt;Structure a comprehensive scheme, incorporating best practices from past successes like Balika Samruddhi, Ladli Laxmi and Chiranjeevi Yojana to support encourage positive attitude amongst families towards the girl child.&lt;/li&gt;
+&lt;li&gt; Program for women healthcare in a mission mode, especially focusing on domains of Nutrition and Pregnancy - with emphasis on rural, SCs, STs and OBCs.&lt;/li&gt;
+&lt;li&gt; We will enable women with training and skills - setting up dedicated Women ITIs, Women wings in other ITIs.&lt;/li&gt;
+&lt;li&gt; Strict implementation of laws related to women, particularly those related to rape.&lt;/li&gt;
+&lt;li&gt; Fund for relief and rehabilitation of rape victims lies unused at the Centre as the Government has
+not worked out the modalities of dispensation. BJP will clear this on priority.&lt;/li&gt;
+&lt;li&gt; Government will create an Acid Attack victims welfare fund to take care of the medical costs related to treatment and cosmetic reconstructive surgeries of such victims.&lt;/li&gt;
+&lt;li&gt; Make police stations women friendly, and increase the number of women in police at different levels.&lt;/li&gt;
+&lt;li&gt; Introduce self defence as a part of the school curriculum.&lt;/li&gt;
+&lt;li&gt; Using information technology for women's safety.&lt;/li&gt;
+&lt;li&gt; Set up an All Women Mobile Bank to cater to women.&lt;/li&gt;
+&lt;li&gt; Special skills training and business incubator park for women.&lt;/li&gt;
+&lt;li&gt; Setting up special business facilitation center for women.&lt;/li&gt;
+&lt;li&gt; Expand and improve upon the network of women / working women hostels.&lt;/li&gt;
+&lt;li&gt; Set up a dedicated W-SME (Women Small and medium enterprises) cluster in every district.&lt;/li&gt;
+&lt;li&gt; Review the working conditions and enhance the remuneration of Anganwadi worker's.&lt;/li&gt;
+&lt;li&gt; Remove any remaining gender disparities in property rights, marital rights and cohabitation rights.&lt;/li&gt;
+ &lt;li&gt;Special adult literacy initiative would be started for women with focus on SCs, STs, OBCs, and slum residents.&lt;/li&gt;
+&lt;li&gt; Will ensure that the loans to Women Self Help Groups would be available at low interest rates.&lt;/li&gt;
+&lt;li&gt; Special programs aimed at girls below poverty line, tribals and indigent women.&lt;/li&gt;
+&lt;li&gt; Appropriate measures would be taken to check female foeticide, dowry, child marriage, trafficking, sexual harassment, rape and family violence.&lt;/li&gt;
+&lt;li&gt;We will transform the quality of life of women in Rural India by providing electricity, tapped water, cleaner fuel and toilets in every home.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>EducationEnrollandExcel</t>
   </si>
   <si>
@@ -694,6 +806,16 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP believes that education is the most powerful tool for the advancement of the nation and the most potent weapon to fight poverty. Education in India needs to be revitalized and reorganized to make future generations proud of their culture, heritage and history and also for creating confidence in the vitality of India. Every effort shall be made to ensure 'equality of opportunity in access and success' to all learners; creating a harmonious, and cohesive egalitarian society that practices democratic values. This would be possible only when Education accords due emphasis on national integration, social cohesion, religious amity, national identity and patriotism. It must also be analyzed how far education has contributed to moral, ethical and humanistic values in the individuals and the society.&lt;/p&gt;
+&lt;p&gt;Education must create minds free from superstitions, hatred and violence and become an important vehicle to cement national unity, social cohesion and religious amity. Our endeavour should be to inculcate moral, ethical and humanistic values in the individuals and the society.&lt;/p&gt;
+&lt;p&gt;India has to become a knowledge society and has to reverberate with educated skilled manpower of high standards required to meet the challenges of 21st century. This requires a bold and visionary leadership to introduce appropriate policy and structural changes.&lt;/p&gt;
+&lt;p&gt;Highest priority would be given to address the acute shortage of teachers and researchers, quality of education and research, and also the employability factor associated with most of the courses. Education should not only lead to employability but also job creation and entrepreneurship by introducing a national multi-skills orientation program.&lt;/p&gt;
+&lt;p&gt;We intend to review and revise education system; the salary structures associated with the teaching staff and most importantly, address the shortfall of faculty and related issues in the country. The system shall be made people-friendly and the credibility of the system shall be restored.&lt;/p&gt;
+&lt;p&gt;Investment in education yields the best dividend. Public spending on education would be raised to 6% of the GDP, and involving the private sector would further enhance this.&lt;/p&gt;
+&lt;p&gt;Under the scheme of 'Quality education for all', BJP would take the following steps.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>SchoolEducation</t>
   </si>
   <si>
@@ -703,6 +825,23 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>&lt;ul&gt;
+ &lt;li&gt;NDA's flagship program 'Sarva Shiksha Abhiyan': Mechanism would be set up for its performance audit and to have real time information about its performance. Programme shall be strengthened and expanded with a goal to remove illiteracy.&lt;/li&gt;
+ &lt;li&gt;Universalization of secondary school education and skills development through functional school shall be seriously pursued with particular focus on rural, tribal and difficult areas.&lt;/li&gt;
+ &lt;li&gt;The content and process of school education shall be thoroughly reviewed to make it dynamic, stress-free, attractive and responsive to the emerging national needs.&lt;/li&gt;
+ &lt;li&gt;Girls shall be provided all possible help to continue and complete school education.&lt;/li&gt;
+ &lt;li&gt;The digital divide shall not be allowed to create further divisions in the learning situations of children.&lt;/li&gt;
+ &lt;li&gt;Special pedagogy would be developed for differently-abled students.&lt;/li&gt;
+ &lt;li&gt;On priority, a national modernization programme for madrasa's would be started.&lt;/li&gt;
+ &lt;li&gt;Mid-day meal scheme would be revitalized in terms of management and delivery.&lt;/li&gt;
+ &lt;li&gt;We will explore ways to reduce the daily burden of carrying books to school for children, which would also entail use of technology for education as a mission mode project.&lt;/li&gt;
+ &lt;li&gt;Establish a national E-Library to empower school teachers and students.&lt;/li&gt;
+ &lt;li&gt;Initiate a multi-country student exchange programme for broadening the horizon of school going
+ children.&lt;/li&gt;
+ &lt;li&gt;Creative talents of students will be recognized and encouraged.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>HigherandProfessionalEducation</t>
   </si>
   <si>
@@ -712,6 +851,24 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;The basic objective of higher and professional education is not only rapid advancement of the affluent sector of the society but also to improve the lot of the last man in the line.&lt;/p&gt;
+&lt;p&gt;The content should be designed to prepare the students to understand the current challenges and equip themselves to be able to readily adjust in a fast changing global scenario. Policy interventions would include:&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;enhancing the pivotal role of the teachers by reworking the work culture of teacher training institutions with a goal to prepare committed and performing teachers.&lt;/li&gt;
+&lt;li&gt; optimum utilization of physical and manpower resources.&lt;/li&gt;
+&lt;li&gt; a mechanism for close interaction between industry (including SME), academia and community
+would be instituted.&lt;/li&gt;
+&lt;li&gt; needs assessment exercise will be done for identifying the future needs across sectors, and the same would be used for developing appropriate courses for higher education, to ensure that the country has adequate manpower for every sector, both established and emerging, in the economy.&lt;/li&gt;
+&lt;li&gt; will provide autonomy with steps to ensure accountability for institutions of higher learning.&lt;/li&gt;
+&lt;li&gt; will raise the standard of education and research, so that Indian universities become at par with
+the top global universities and find their place in the global league.&lt;/li&gt;
+&lt;li&gt; the credibility of the regulatory bodies shall be restored. The procedures to make appointments to senior positions shall be made transparent and merit and ability shall be the sole criterion.&lt;/li&gt;
+&lt;li&gt; UGC will be restructured and it will be transformed into a Higher Education Commission rather than just being a grant distribution agency.&lt;/li&gt;
+&lt;li&gt; we will revisit the Apprenticeship Act to facilitate our youth to Earn while they Learn.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>VocationalTraining</t>
   </si>
   <si>
@@ -721,6 +878,15 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;ul&gt;
+ &lt;li&gt;Would set up Massive Open Online Courses (MOOC) and virtual classrooms to make it convenient for working class people and housewives to further their knowledge and qualifications.&lt;/li&gt;
+ &lt;li&gt;Correspondence courses will be started in new domains for self-employment, family run businesses, entrepreneurship and innovation, and these courses would be provided for free to women. The goal would be to prepare the youth for jobs being created by the emerging sectors, foster a spirit of innovation and entrepreneurship, leading to more incomes and job creation.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;BJP will set up a National Commission on Education to report in two years on the state of education and the reforms needed. Based on the report, BJP will implement a National Education Policy to meet the changing dynamics of the population's requirement with regards to quality education, innovation and research, aiming to make India a knowledge superpower by equipping its students with the necessary skills and knowledge and to eliminate the shortage of manpower in science, technology, academics and industry.&lt;/p&gt;
+</t>
+  </si>
+  <si>
     <t>SkillsFocusingonProductivityandEmployability</t>
   </si>
   <si>
@@ -730,6 +896,29 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Skillful hands, bright minds, discipline and perseverance makes Indian talent an asset worldwide. We have to live up to this potential, preparing the World's Largest Workforce. We have to make our youth productively employed and gainfully engaged. We also have to develop India as a Knowledge Powerhouse. We have to train and nurture our human resource. We have to use it for leap-frogging our Nation into the future. Unfortunately, the initiatives taken by Congress for this have fallen woefully short, being almost non-starters.
+&lt;/p&gt;
+&lt;p&gt;We will take up skill development on a mission mode, at an unprecedented scale.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Skill Mapping - to help scientifically plan our national human resource development that India would need (like engineers, architects, doctors, nurses, lawyers, accountants, plumbers, carpenters, welders, etc.).&lt;/li&gt;
+&lt;li&gt; Launch a 'National Multi-skill Mission'&lt;/li&gt;
+&lt;li&gt; We will run short-term courses, in the evenings, focusing on employable skills.&lt;/li&gt;
+&lt;li&gt; We will also set up Centres of Excellence in various sectors in partnership with the Industry.&lt;/li&gt;
+&lt;li&gt; To ensure industry responsive manpower, we will bring together industry, universities and government.&lt;/li&gt;
+&lt;li&gt; We will promote vocational training on a massive scale. Rigid segregation of formal education and skill development will be broken; a mechanism will be established to give vocational qualifications of Academic Equivalence.&lt;/li&gt;
+&lt;li&gt; We will also create institutional mechanisms to refresh and upgrade abilities through continuing education - to make them employable.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;We will focus on need based skill development and employability; making our youth employable even in the most sophisticated jobs.&lt;/p&gt;
+&lt;p&gt;We will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; put emphasis on imparting soft skills to enhance employability including a national program on foreign languages.&lt;/li&gt;
+&lt;li&gt; launch a national programme for digital empowerment through computer literacy of the people, especially the youth.&lt;/li&gt;
+&lt;li&gt; we will assess the talent and capacity of our youth from an early age; so they can be groomed accordingly.&lt;/li&gt;
+&lt;li&gt; we will push for greater practical and research training encouraging real world experience through internships and apprenticeships.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>HealthServicesIncreasetheAccessImprovetheQualityLowertheCost</t>
   </si>
   <si>
@@ -739,6 +928,45 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;India needs a holistic care system that is universally accessible, affordable and effective and drastically reduces the out of pocket spending on health. NRHM has failed to meet the objectives and will be radically reformed. BJP accords high priority to health sector, which is crucial for securing the economy.&lt;/p&gt;
+&lt;p&gt;The overarching goal of healthcare would be to provide, 'Health Assurance to all Indians and to reduce the out of pocket spending on health care', with the help of state governments.&lt;/p&gt;
+&lt;p&gt;The current situation calls for radical reforms in the healthcare system with regards to national healthcare programs and delivery, medical education and training and financing of healthcare. Our government would focus on the following reforms in healthcare:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; the last healthcare policy dates back to 2002. India now needs a comprehensive healthcare policy to address the complex healthcare challenges, keeping in view the developments in the healthcare sector and the changing demographics. BJP will initiate the New Health Policy.&lt;/li&gt;
+&lt;li&gt; initiate the 'National Health Assurance Mission', with a clear mandate to provide universal healthcare that is not only accessible and affordable, but also effective, and reduces the OOP spending for the common man.&lt;/li&gt;
+&lt;li&gt; Education and Training - Will review the role of various professional regulatory bodies in healthcare and consider setting up an overarching lean body for healthcare. High priority will be given to address the shortfall of healthcare professionals.&lt;/li&gt;
+&lt;li&gt; Modernize Government hospitals, upgrading infrastructure and latest technologies.&lt;/li&gt;
+&lt;li&gt; Reorganize Ministry of Health and Family Welfare in order to converge various departments dealing
+in healthcare, food and nutrition and pharmaceuticals, for effective delivery of healthcare services.&lt;/li&gt;
+&lt;li&gt; Increase the number of medical and para-medical colleges to make India self sufficient in human resources, and set up an AIIMS like institute in every state.&lt;/li&gt;
+&lt;li&gt; Yoga and Ayurveda are the gifts of ancient Indian civilization to humanity and we will increase the public investment to promote Yoga and AYUSH. We will start integrated courses for Indian System of Medicine (ISM) and modern science and Ayurgenomics. We will set up institutions and launch a vigorous program to standardize and validate the Ayurvedic medicine.&lt;/li&gt;
+&lt;li&gt; Move to pre-emptive care model where the focus and thrust will be on child health and prevention.&lt;/li&gt;
+&lt;li&gt; School health program would be a major focus area, and health and hygiene will be made a part of
+the school curriculum.&lt;/li&gt;
+&lt;li&gt; Focus on Rural Health care delivery.&lt;/li&gt;
+&lt;li&gt; Senior Citizens healthcare would be a special focus area.&lt;/li&gt;
+&lt;li&gt; Give high priority to chronic diseases, and will invest in research and development of solutions for chronic diseases like obesity, diabetes, cancer, CVD etc.&lt;/li&gt;
+&lt;li&gt; Occupational health programs will be pursued aggressively.&lt;/li&gt;
+&lt;li&gt; Utilize the ubiquitous platform of mobile phones for healthcare delivery and set up the 'National eHealth Authority' to leverage telemedicine and mobile healthcare for expanding reach and coverage and to define the standards and legal framework for technology driven care.&lt;/li&gt;
+&lt;li&gt; Universalization of emergency medical services-108.&lt;/li&gt;
+&lt;li&gt; Re-orientation of herbal plants board to encourage farming of herbal plants.&lt;/li&gt;
+&lt;li&gt; Population stabilization would be a major thrust area and would be pursued as a mission mode program.&lt;/li&gt;
+&lt;li&gt; Programme for Women Healthcare with emphasis on rural, SC, ST and OBC in a mission mode.&lt;/li&gt;
+&lt;li&gt; Mission mode project to eradicate malnutrition.&lt;/li&gt;
+&lt;li&gt; Launch National Mosquito Control mission.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Poor Hygiene and Sanitation have a far reaching, cascading impact. We will ensure a 'Swachh Bharat' by Gandhiji's 150th birth anniversary in 2019, taking it up in mission mode by converging resources and building around jan bhagidari:
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Create an open defecation free India by awareness campaign and enabling people to build toilets in their home as well as in schools and public places.&lt;/li&gt;
+&lt;li&gt; Set up modern, scientific sewage and waste management systems.&lt;/li&gt;
+&lt;li&gt; We will introduce Sanitation Ratings measuring and ranking our cities and towns on 'sanitation';
+and rewarding the best performers.&lt;/li&gt;
+&lt;li&gt; Make potable drinking water available to all thus reducing water-borne diseases, which will automatically translate into Diarrhoea-free India.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>EconomicRevival</t>
   </si>
   <si>
@@ -748,6 +976,23 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;When the NDA Government completed its tenure the baton was handed over to the incoming UPA Government with GDP growth nearing double digit in 2004. Inflation was under control. Fiscal Deficit and Current Account Deficit were kept within limit and the overall Economy was showing robust fundamentals. In contrast, now at the end of Congress-led UPA regime, the GDP growth has plummeted to very low of 4.8%, the inflation and price rise beyond control, the fiscal deficit and current account deficit in the alarm zone, and the manufacturing sector facing a recession. The Congress-led UPA has indulged in massive scams during its last five years. In recent years, the Indian Rupee has seen a free fall like never before.&lt;/p&gt;
+&lt;p&gt;This is basically the result of policy and decision paralysis of the UPA Government. Decisions are simply not taken. And if they are taken, they turn into scandals. All this has destroyed the reputation of our economy. To reverse this process, the first thing, which is required, is to restore confidence in the integrity of the decision-making and sanctity of our decisions.&lt;/p&gt;
+&lt;p&gt;We will bring back credibility and trust in government, re-sowing confidence in the India story domestically as well as internationally. Through consistent, long-term policies, we will not just spur the process of economic growth, but also ensure that it is stable as well as balanced.&lt;/p&gt;
+&lt;p&gt;We will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; find out solutions, which are effective in the short run and lasting in the long run.&lt;/li&gt;
+&lt;li&gt; strictly implement Fiscal discipline, without compromising on funds availability for development work and asset creation&lt;/li&gt;
+&lt;li&gt; allocate resources efficiently and effectively to re-energize the engines of growth.&lt;/li&gt;
+&lt;li&gt; re-visit the policy framework for investments both foreign and domestic to make them more
+conducive.&lt;/li&gt;
+&lt;li&gt; undertake Banking reforms to enhance ease and access, as well as accountability.&lt;/li&gt;
+&lt;li&gt; we will encourage Savings as an important driver of investment and growth.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>NPAs</t>
   </si>
   <si>
@@ -757,6 +1002,9 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>NPAs have increased sharply over the past few years and the trend continues. BJP will take necessary steps to reduce NPAs in Banking sector. Also, BJP will set up a strong regulatory framework for the non-banking financial companies to protect the investors.</t>
+  </si>
+  <si>
     <t>Taxation</t>
   </si>
   <si>
@@ -766,6 +1014,17 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;UPA Government has unleashed 'Tax terrorism' and 'uncertainty', which not only creates anxiety amongst the business class and negatively impacts the investment climate, but also dents the image of the country. BJP realizes the importance of having a Tax Policy Roadmap, so that people are aware of the future and plan accordingly. We will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; provide a non adversarial and conducive tax environment&lt;/li&gt;
+&lt;li&gt; rationalize and simplify the tax regime&lt;/li&gt;
+&lt;li&gt; overhaul the dispute resolution mechanisms&lt;/li&gt;
+&lt;li&gt; bring on board all State governments in adopting GST, addressing all their concerns&lt;/li&gt;
+&lt;li&gt; provide tax incentives for investments in research and development, geared towards indigenization of technology and innovation&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>ForeignDirectInvestment</t>
   </si>
   <si>
@@ -775,6 +1034,9 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>Barring the multi-brand retail sector, FDI will be allowed in sectors wherever needed for job and asset creation, infrastructure and acquisition of niche technology and specialized expertise. BJP is committed to protecting the interest of small and medium retailers, SMEs and those employed by them. The FIPBs (Foreign Investment Promotion Board) functioning shall be made more efficient and investor- friendly</t>
+  </si>
+  <si>
     <t>AgricultureProductiveScientificandRewarding</t>
   </si>
   <si>
@@ -784,6 +1046,40 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Agriculture is the engine of India's economic growth and the largest employer, and BJP commits highest priority to agricultural growth, increase in farmer's income and rural development.&lt;/p&gt;
+&lt;p&gt;BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; increase public investment in agriculture and rural development.&lt;/li&gt;
+&lt;li&gt; take steps to enhance the profitability in agriculture, by ensuring a minimum of 50% profits over the cost of production, cheaper agriculture inputs and credit; introducing latest technologies for farming and high yielding seeds and linking MGNREGA to agriculture.&lt;/li&gt;
+&lt;li&gt; Put in place welfare measures for farmers above 60 years in age, small and marginal farmers and farm labours.&lt;/li&gt;
+&lt;li&gt; Introduce and promote low water consuming irrigation techniques and optimum utilization of water resources.&lt;/li&gt;
+&lt;li&gt; Introduce soil assessment based crop planning and setting up mobile soil testing labs.&lt;/li&gt;
+&lt;li&gt; Re-orient pest management and control programmes.&lt;/li&gt;
+&lt;li&gt; implement and incentivize the setting up of the food processing industry that has remained just a plain talk till now. This will lead to better income for farmers and create jobs. We aim to set up 'agro food processing clusters', with high value, export-quality and vacuum packed food processing facilities, etc.&lt;/li&gt;
+&lt;li&gt; Focus on the quality, productivity and trade of spices.&lt;/li&gt;
+&lt;li&gt; Set up the 'Organic Farming and Fertilizer Corporation of India', to promote organic farming and
+fertilizers, and provide incentives and support for marketing organic produce.&lt;/li&gt;
+&lt;li&gt; Introduce rotation farming for herbal products, based on geographical mapping, to enhance the income of farmers.&lt;/li&gt;
+&lt;li&gt; Implement a farm insurance scheme to take care of crop loss due to unforeseen natural calamities.&lt;/li&gt;
+&lt;li&gt; Strengthen and expand rural credit facilities.&lt;/li&gt;
+&lt;li&gt; Promote horticulture, floriculture, pisciculture, bee-keeping and poultry for generating jobs and income for rural India&lt;/li&gt;
+&lt;li&gt; Promote fish farming and aqua culture. Measures would be taken for the welfare of fisherman&lt;/li&gt;
+&lt;li&gt; Create Cluster based storage systems (e.g. Rice cluster, Wheat Cluster, Veg - Fruit cluster,
+Spices cluster).&lt;/li&gt;
+&lt;li&gt; Introduce the concept of consumer friendly farmers' market to reduce wastages and increase incomes and risk coverage.&lt;/li&gt;
+&lt;li&gt; Reform the APMC act.&lt;/li&gt;
+&lt;li&gt; Work with the states to set up seed culture labs in each district and regional agriculture innovation
+labs to conserve agro-biodiversity and to identify and preserve rare indigenous varieties.&lt;/li&gt;
+&lt;li&gt; Explore setting up of regional Kisan TV channels.&lt;/li&gt;
+&lt;li&gt; Give high priority to poverty alleviation in rural areas.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Genetically Modified (GM) foods will not be allowed without full scientific evaluation on its long-term effects on soil, production and biological impact on consumers.&lt;/p&gt;
+&lt;p&gt;
+Land acquisition is a contentious issue due to the opacity of the land acquisition process. BJP will adopt a 'National Land Use Policy', which will look at the scientific acquisition of non-cultivable land, and its development; protect the interest of farmers and keep in mind the food production goals and economic goals of the country. It's implementation would be monitored by the National Land Use Authority, which will work with the State Land Use Authorities to regulate and facilitate land management. The power and functions of the National Land Use Authority would be similar to those of other regulatory bodies.&lt;/p&gt;
+</t>
+  </si>
+  <si>
     <t>IndustryModernCompetitiveandCaring</t>
   </si>
   <si>
@@ -793,6 +1089,24 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;We should no longer remain a market for the global industry. Rather, we should become a Global Manufacturing Hub. We have to encourage our industry to innovate and collaborate internationally. We have to encourage industry to produce efficiently and cost-effectively.&lt;/p&gt;
+&lt;p&gt;Economic freedom implies that Government will not get in the way of the freedom of individuals to start and operate legitimate businesses. Increased economic freedom will break open the economic space to new entrants, especially in the form of small and medium-enterprises, creating jobs and prosperity. Particularly:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; We will ensure that a conducive, enabling environment is created making 'doing business' in India easy.&lt;/li&gt;
+&lt;li&gt; We will focus on cutting the red tape, simplifying the procedures and removing the bottle- necks.&lt;/li&gt;
+&lt;li&gt; We will ensure logistics infrastructure, including stable power.&lt;/li&gt;
+&lt;li&gt; Our attempt will be to move towards a single-window system of clearances both at the centre
+and also at the State level through a Hub-spoke model.&lt;/li&gt;
+&lt;li&gt; We will put in place a mechanism that will ensure that the Central and state governments work in close coordination and synergy while giving clearances to mega projects.&lt;/li&gt;
+&lt;li&gt; Decision-making on environment clearances will be made transparent as well as time-bound.&lt;/li&gt;
+&lt;li&gt; We will set up World class Investment and Industrial regions as Global Hubs of Manufacturing.&lt;/li&gt;
+&lt;li&gt; We will set up a task force to review and revive our MSME sector (Micro and Small Medium scale Enterprises); enabling it with better access to formal credit and technology for modernization.&lt;/li&gt;
+&lt;li&gt; Frame the environment laws in a manner that provides no scope for confusion and will lead to speedy clearance of proposals without delay.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>Manufacturing</t>
   </si>
   <si>
@@ -802,6 +1116,21 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;A strong manufacturing sector will not only bridge the demand-supply gap leading to price stabilization, but also create millions of jobs and increase incomes for the working class. Above all, it will increase the revenue for government and lead to import substitution to bring down the import bill. We will make India a hub for cost-competitive labour-intensive mass manufacturing. To give boost to manufacturing, BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Accord high priority to the growth of manufacturing, so that we can create enough jobs in the country. This sector must grow fast to ensure employment and asset creation.&lt;/li&gt;
+&lt;li&gt; Take steps for Interest rate rationalization and have a clear tax policy to remove uncertainty and create investor confidence.&lt;/li&gt;
+&lt;li&gt; Take all steps; like removing red-tapism involved in approvals, to make it easy to do business, invest in logistics infrastructure, ensure power supply and undertake labour reforms, besides other steps to create a conducive environment for investors.&lt;/li&gt;
+&lt;li&gt; Increase the public spending on R&amp;amp;D and Incentivize R&amp;amp;D investments by the industry to increase the competitiveness of the manufacturing sector.&lt;/li&gt;
+&lt;li&gt; We will facilitate setting up of software and hardware manufacturing units.&lt;/li&gt;
+&lt;li&gt; Encourage Indian companies to go global and we will support Indian companies in this endeavor. We believe that Indian entrepreneurs have the capability to take on global markets.&lt;/li&gt;
+&lt;li&gt; Set up trade facilitation to ensure easier customs clearances and visas for business travel.&lt;/li&gt;
+&lt;li&gt; Initiate a Government - Industry Dialogue, a channel for regular interface with the industry.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>MSMEsMicrosmallandmediumenterprises</t>
   </si>
   <si>
@@ -811,6 +1140,9 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>BJP considers that the role of SME sector is crucial for the economic development of our country. The sector needs to be developed by providing international linkages for exports, availability of credit through a dedicated SME bank, supply chain efficiencies, adoption of IT, support in R&amp;D and innovation, and a policy support for enhancing the mandate to purchase from SME for large scale projects. Overall goal is to enhance the competitiveness of the SME sector leading to a larger contribution to our economic growth and employment generation.</t>
+  </si>
+  <si>
     <t>CooperativeSector</t>
   </si>
   <si>
@@ -820,6 +1152,9 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>Every effort will be made to encourage the cooperative sector. BJP commits to review the existing laws with regards to the cooperative sector, and will amend the multi-state cooperative act to remove lacunae and anomalies.</t>
+  </si>
+  <si>
     <t>Handicrafts</t>
   </si>
   <si>
@@ -829,6 +1164,15 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;We will move up the value chain of the sector driven by a focus on Quality.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Market linkages - both national and international&lt;/li&gt;
+&lt;li&gt; Access to credit and information and skills upgradation&lt;/li&gt;
+&lt;li&gt; Value addition will be encouraged through avenues like - branding, packaging and technology.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>Artisans</t>
   </si>
   <si>
@@ -838,6 +1182,9 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>Schemes will be drawn for skills upgradation and enhancement of business opportunities for artisans like smiths, weavers, carpenters, hair-dressers, shoe-smiths, and potters.</t>
+  </si>
+  <si>
     <t>ServicesDrivenbyQualityandEfficiency</t>
   </si>
   <si>
@@ -856,6 +1203,27 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;The modern era is an era of exchange. Over-regulation needs to be addressed to stop the harassment of the businessmen and traders. At the same time, we have to set up transparent systems, which ensure credibility of our goods and services. At the same time, the bottlenecks in transporting and exporting them have to be removed. Also, the flow of information about our tradable items has to be made available to the rest of the world.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Focus on Zero defect products.&lt;/li&gt;
+&lt;li&gt; Build world class Ports; connecting them with roads and rail to the hinterland so as to drive the
+maritime trade of the country.&lt;/li&gt;
+&lt;li&gt;Air Cargo facilities will be enhanced throughout the country.&lt;/li&gt;
+&lt;li&gt; An Export Promotion Mission will be established integrating all stakeholders.&lt;/li&gt;
+&lt;li&gt; Current accounts deficit will be brought down aggressively by focusing on exports and reducing the dependency on imports. Value addition on our products will be the biggest task.&lt;/li&gt;
+&lt;li&gt; We shall work with the State governments to usher in the GST in an appropriate timeframe. For implementing the same, a robust IT network system will be put in place.&lt;/li&gt;
+&lt;li&gt; We will embark on the path of IPRs and Patents in a big way.&lt;/li&gt;
+&lt;li&gt; Take all necessary steps to protect the interest of retailers, small traders and small vendors and equip them with the latest techniques and methods to modernize them and make them competitive.&lt;/li&gt;
+&lt;li&gt; Commit to ensure that the retailers and SMEs don't have to spend time and money for seeking multiple licenses to start the business. There will a system in place to avoid harassment of small traders.&lt;/li&gt;
+&lt;li&gt;Ensure easy availability of institutional credit.&lt;/li&gt;
+&lt;li&gt; Review obsolete and multiple laws to reduce and simplify them.&lt;/li&gt;
+&lt;li&gt; Remove ambiguity in rules to make way for prompt decisions without any scope for discretion.&lt;/li&gt;
+&lt;li&gt; Telecom revolution has touched length and breadth of the country but there is significant scope and necessity to improve the quality of voice and data to fully leverage the potential.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>TourismUntappedPotential</t>
   </si>
   <si>
@@ -865,6 +1233,11 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>&lt;p&gt;BJP recognizes the role tourism and hospitality can play as a foreign exchange earner and its ability to create millions of jobs every year. Tourism plays a key role in socio-economic progress through creation of jobs, enterprise, infrastructure development, and foreign exchange earnings.&lt;/p&gt;
+&lt;p&gt;BJP realizes that the tourism sector needs a clear plan for growth, and BJP commits to initiate a mission mode project to create 50 tourist circuits that are affordable and built around themes like: a.) Archaeological and Heritage, b.) Cultural and Spiritual, c.) Himalayan, d.) Desert, e.) Coastal, f.) Medical (Ayurveda and Modern Medicine), etc. This will lead to creation of infrastructure and employment around each tourist circuit and help in boosting revenue generation.&lt;/p&gt;
+&lt;p&gt;Specialized course in tourism will be started for capacity development. Safety and Security of tourists would be accorded due priority.&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>LabourForceThePillarofOurGrowth</t>
   </si>
   <si>
@@ -874,6 +1247,18 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP recognizes the fact that the labour is the key to the revival of the economy and so are the laws governing them. We believe in promoting a harmonious relationship between labour and the industry, with both playing an important contributory role in economic growth and development.&lt;/p&gt;
+&lt;p&gt;We will ensure that the interests of labour in the unorganized sector are protected.&lt;/p&gt;
+&lt;p&gt;For the organized labour, we propose to encourage industry owners and labour to embrace the concept of 'Industry Family'. This concept, in which industry owners and labours bond as a family, is guided by the principles of efficiency, skill development and upgradation, productivity, appropriate wages and perquisites, and security towards this end. We will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; issue identity cards to the unorganized sector labourers, and arrangements will be made to provide them good quality health and education services. Also, their skills will be upgraded through appropriate training programs.&lt;/li&gt;
+&lt;li&gt; extend access to modern financial services to labour - including considering the option of setting up a dedicated Workers Bank.&lt;/li&gt;
+&lt;li&gt; bring together all stakeholders to review our Labour laws which are outdated, complicated and even contradictory.&lt;/li&gt;
+&lt;li&gt; strengthen the Pension and Health Insurance safety nets for all kinds of labourers.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>HousingNoLongeraMirage</t>
   </si>
   <si>
@@ -883,6 +1268,18 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;We will roll out a massive Low cost Housing programme to ensure that by the time the nation completes 75 years of its Independence, every family will have a pucca house of its own. It will be an innovatively designed scheme that dovetails various existing programmes and also encourages the housing sector by appropriate policy interventions and credit availability including interest subventions, where necessary.&lt;/p&gt;
+&lt;p&gt;Our proposed programme will further ensure that these houses are equipped with the basic facilities of toilet, piped water supply, electricity and proper Access. To do this we will amongst others:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Prioritize all our resources towards this goal.&lt;/li&gt;
+&lt;li&gt; Leverage on land as a resource in urban areas and demand for unskilled labour in the rural areas.&lt;/li&gt;
+&lt;li&gt; Innovatively structure the programme to converge and dovetail various existing programmes, while adding the missing links.&lt;/li&gt;
+&lt;li&gt; Simultaneously encourage the overall housing sector, through appropriate policy interventions and credit availability and interest subvention schemes.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>PhysicalInfrastructureBetterthantheBest</t>
   </si>
   <si>
@@ -892,6 +1289,21 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;India should no longer be limited by its infrastructure. In fact, we have to create robust infrastructure, which drives growth. For this purpose, we have to devote ourselves for a decade. We have to think big. Also, looking to the expansion in our population as well as social and economic activities, we have to build our infrastructure in a futuristic way. Growth of this sector means the growth of cement, steel, electricity and many other associated industries and directly leads to massive job creation. To achieve this, we will take following steps.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Work on the Freight Corridors and attendant Industrial Corridors will be expedited. This will result in the faster movement of people and goods.&lt;/li&gt;
+&lt;li&gt; Remote states like those in the Northeast and Jammu and Kashmir will be connected with the rest of India through world class highways and rail lines.&lt;/li&gt;
+&lt;li&gt; National Highway construction projects will be expedited, especially Border and Coastal highways.&lt;/li&gt;
+&lt;li&gt; Every village will be connected through all-weather roads.&lt;/li&gt;
+&lt;li&gt; We shall modernize existing and operational Airports, and build new ones especially connecting smaller towns and all tourism circuits. In addition, there is a potential for inland air transportation to various remote and local locations in the country. Such air strips will be developed so that low cost air travelling becomes possible within the country.&lt;/li&gt;
+&lt;li&gt; We will evolve an economic model of Port-led development. India is blessed with a long coastline. We will modernize existing ports on one hand, and develop new ones on the other - stringing together our Sagar Mala project.&lt;/li&gt;
+&lt;li&gt; Public Private Partnership would be encouraged to tap into private sector resources as well as expertise. An institutional framework would be established for the same; while regulators would be given greater autonomy as well as accountability.
+&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>NextGenerationInfrastructure</t>
   </si>
   <si>
@@ -901,6 +1313,16 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;We will:&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;set up Gas Grids to make gas available to households and industry.&lt;/li&gt;
+ &lt;li&gt;set up a National Optical-Fibre Network up to the village level; and Wi-Fi zones in public areas.&lt;/li&gt;
+ &lt;li&gt;harness our advanced satellite technology and expertise for development.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>Transport</t>
   </si>
   <si>
@@ -910,6 +1332,17 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;The BJP realizes the importance of travel for the vibrancy of the economy and social unity. BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Create a public transport system, which can reduce the dependence on personal vehicles for transport, thereby, reducing cost, time to travel as well as ecological cost.&lt;/li&gt;
+&lt;li&gt; Launch an Integrated Public transport project which will include roadways, railways and waterways.&lt;/li&gt;
+&lt;li&gt; Develop waterways for passenger and cargo transport.&lt;/li&gt;
+&lt;li&gt; Develop National logistics network for faster movement of goods.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>Railway</t>
   </si>
   <si>
@@ -919,6 +1352,22 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Indian Railways is the lifeline of the country. It will be modernized, strengthened and upgraded to serve passengers as well as the country's economy. This will be done in a planned manner focusing on national development, rather than political exigency.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Hinterland will be connected to the ports through strategic new Rail networks.&lt;/li&gt;
+&lt;li&gt; Agri Rail network will be established - with Train Wagons designed to cater to the specific needs of perishable Agricultural products like milk and vegetables as well as light weight wagons for salt movement.&lt;/li&gt;
+&lt;li&gt; Tourist Rail - including Pilgrimage Rail.&lt;/li&gt;
+&lt;li&gt; Railways Modernization, inducting of state-of-the-art technology.&lt;/li&gt;
+&lt;li&gt; Special focus on developing skilled human resources to meet future demand.&lt;/li&gt;
+&lt;li&gt;Prioritize Safety and invest in long required overhaul of stressed infrastructure, strict norms and warning systems.&lt;/li&gt;
+&lt;li&gt; Modernize and equip all stations with requisite infrastructure and public utilities.&lt;/li&gt;
+&lt;li&gt; Convert all unmanned crossings into manned crossings in a phased manner.&lt;/li&gt;
+&lt;li&gt; Initiate R&amp;amp;D for indigenous railways, coach design and signals.&lt;/li&gt;
+&lt;li&gt; We will launch Diamond Quadrilateral project - of High Speed Train network (bullet train).&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>WaterMakeItReachtoAllHomesFarmsandFactories</t>
   </si>
   <si>
@@ -928,6 +1377,25 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Trends indicate that India would be a 'water stressed' state by 2050, and the gap between the demand and supply would be 50%. BJP recognizes the seriousness of the issue. Also, most importantly, potable drinking water is not available to the entire population despite more than six decades of independence. Water is a dwindling resource, with the threat of water scarcity looming large. We will address this in a comprehensive manner across multiple dimensions. BJP remains committed to giving high priority to water security.&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Launch the 'Pradhan Mantri Gram Sinchayee Yojana' with a motto of 'har khet ko paani'. We will launch multi-pronged 'water strategy' for reducing farmer's dependence on monsoon. Increase irrigated land by completing the long pending irrigation projects on priority.&lt;/li&gt;
+&lt;li&gt; We will nurture ground water recharge harnessing rain water to reduce dependence on ground water.&lt;/li&gt;
+&lt;li&gt; Encourage efficient use, water conservation, recycling and rain water harvesting.&lt;/li&gt;
+&lt;li&gt; Sewage treatment plants to prevent the pollution of rivers.&lt;/li&gt;
+&lt;li&gt; Desalination plants for drinking water supply in coastal cities.&lt;/li&gt;
+&lt;li&gt; Inter-linking of rivers based on feasibility.&lt;/li&gt;
+&lt;li&gt; Examination of ground water to eliminate toxic chemicals, particularly arsenic and fluorides.&lt;/li&gt;
+&lt;p&gt;To ensure drinking water security to all. We will:&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Encourage setting up of drinking water supply grid in water scarce areas.&lt;/li&gt;
+&lt;li&gt; Promote decentralized, demand-driven, community-managed water resource management, water supply and environmental sanitation.&lt;/li&gt;
+&lt;li&gt; Facilitate piped water to all households.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>EnergyGenerateMoreUseRationallyWasteLess</t>
   </si>
   <si>
@@ -937,6 +1405,20 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP realizes the need to focus on generation and distribution of power as a national security issue, so that the growth is not negatively impacted due to supply issues in the energy sector. The overarching goal of energy security is to ensure affordable energy for various consumer segments. Steps will be taken to avoid over- dependence on any one fuel and ensure supplier diversity, to avoid reliance on one supplier, country and developing indigenous capacities to meet the emerging needs.&lt;/p&gt;
+&lt;p&gt;BJP will:&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Come out with a responsible and comprehensive 'National Energy Policy'.&lt;/li&gt;
+&lt;li&gt; Focus on development of energy infrastructure, human resource development and upgradation of technology.&lt;/li&gt;
+&lt;li&gt; Take steps to maximize the potential of oil, gas, hydel power, ocean, wind, coal and nuclear sources. BJP considers energy efficiency and conservation crucial to energy security.&lt;/li&gt;
+&lt;li&gt; Set up small-hydro power generation projects to harness the hydropower that is not being used at the moment. Small projects can be set up with local support and without displacement of the local population.&lt;/li&gt;
+&lt;li&gt; Take Steps to increase the domestic coal exploration and production, to bridge the demand and supply gap. Oil and gas explorations would also be expedited in the country. This will also help to reduce the import bill.&lt;/li&gt;
+&lt;li&gt; Give a thrust to renewable sources of energy as an important component of India's energy mix.&lt;/li&gt;
+&lt;li&gt; Expand and strengthen the national solar mission.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>ScienceandTechnologyIndiaInnovatesandIndiaLeads</t>
   </si>
   <si>
@@ -946,6 +1428,37 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;
+India has been a knowledge economy and has been a leader in science and technology from the ancient times. India now needs policies and programs to reclaim its global leadership position in science and technology. BJP recognizes the need to create an ecosystem for fundamental research and innovation, keeping the objective of science with a human face in the service of the common man. Science and technology has enormous potential to bridge the disparities between the urban and rural India, rich and poor. Scientific education and technology needs to be encouraged, promoted, practiced and leveraged with renewed vision and vigour.&lt;/p&gt;
+&lt;p&gt;BJP recognizes the central role of science and technology in raising the quality of life of the people of the country, particularly of the disadvantaged sections of society in creating wealth for all, in making India globally competitive, in utilizing natural resources in a sustainable manner, in protecting the environment and ensuring national security. We will also encourage and incentivize private sector investments - both domestic and foreign, in science and technology and in high-end research aimed towards innovation.&lt;/p&gt;
+&lt;p&gt;We will focus on the following:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; ensuring food, agricultural, nutritional and environmental, wealth, health and energy security of the people on a sustainable basis, using science and technology.&lt;/li&gt;
+&lt;li&gt; mounting a direct and sustained effort on the alleviation of poverty, enhancing livelihood security, removal of hunger and malnutrition, reduction of drudgery and regional imbalances, both rural and urban, and generation of employment, by using scientific and technological capabilities along with our traditional knowledge pool.&lt;/li&gt;
+&lt;li&gt; encouraging research and innovation in areas of relevance for the economy and society, particularly by promoting close and productive interaction between private and public institutions. Sectors such as agriculture (particularly soil, water management, human and animal nutrition and fisheries), water, health, education, industry, energy including renewable energy, communication and transportation would be accorded highest priority. Leveraging of technologies such as information technology, biotechnology and material sciences would be done with special importance.&lt;/li&gt;
+&lt;li&gt; encouraging research and application to meet the challenges of climate change and for forecasting, prevention and mitigation of natural hazards, particularly floods, cyclones, earthquakes, drought and landslides.&lt;/li&gt;
+&lt;li&gt; promoting international science and technology cooperation towards achieving the goals of national development and security, and making it a key element of our international relations.&lt;/li&gt;
+&lt;li&gt; devise schemes, programs and opportunities to encourage the youth to take scientific research and innovation as a career.&lt;/li&gt;
+&lt;li&gt; provide work environment and professional opportunities in fundamental scientific research, to make research careers more appealing, so that the nation can harness the best of brains for scientific research leading to enhancing the national productivity and competitiveness and reverse brain drain.&lt;/li&gt;
+&lt;li&gt; build world class, regional centres of excellence of scientific research in the field of nanotechnology, material sciences, thorium technology and brain research.&lt;/li&gt;
+&lt;li&gt; create an ecosystem for multi-country and inter-disciplinary collaborative research, and establish an Intellectual Property Rights Regime which maximizes the incentive for generation and protection of intellectual property for all type of inventors.&lt;/li&gt;
+&lt;li&gt; achieving synergy between industry and scientific research. Autonomous technology transfer organizations will be created as associate organizations of universities and national laboratories to transfer the know-how generated by them to industry. Industry will be encouraged to adopt or support educational and research institutions to help direct science and technology endeavours towards tangible industrial goals.&lt;/li&gt;
+&lt;li&gt; promotion of innovation by creating a comprehensive national system of innovation.&lt;/li&gt;
+&lt;li&gt; indigenous knowledge, based on our long and rich tradition will be further developed and harnessed
+for the purpose of wealth and employment generation&lt;/li&gt;
+&lt;li&gt; to promote science popularization schemes extensively.&lt;/li&gt;
+&lt;li&gt; bring the changes in secondary education to focus on application of science.&lt;/li&gt;
+&lt;li&gt; set an institute of Big data and Analytics for studying the impact of big data across sectors for predictive science.&lt;/li&gt;
+&lt;li&gt; to do research for the eradication of tropical diseases.&lt;/li&gt;
+&lt;li&gt; Establish institutes of Technology for Rural Development.&lt;/li&gt;
+&lt;li&gt; establish a Central University dedicated to Himalayan Technology.&lt;/li&gt;
+&lt;li&gt;promote research and application of nuclear science in medicines, industry and agriculture.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;We believe science and technology should be used to build a new and resurgent India that continues to maintain its strong democratic and spiritual traditions, that remains secure not only militarily but also socially and economically. Our science and technology policy will be framed and implemented so as to be in harmony with our worldview of the large human family. We will ensure that science and technology truly uplifts the Indian people and indeed all humanity.
+&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>FloraFaunaandEnvironmentSafeguardingOurTomorrow</t>
   </si>
   <si>
@@ -955,6 +1468,27 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;The present generation has to make this world a better place to live. A better place not only for us, but for our future generations as well. We have to nurture the environment, institutions, people, resources and amenities. We have to combine the past, the present and the future. We have to have a holistic view of human life for sustainable development.&lt;/p&gt;
+&lt;p&gt;We have to develop the assets and amenities for ourselves in a manner that leaves an equally good or even better environment for the future generations. We will put sustainability at the centre of our thoughts and actions, working on the principle that inclusive growth cannot be limited by the barriers of time and space - it has to be built on the foundations of the past, leverage on the opportunities of the present, and preserve and enhance its resources for the future. We will take Climate Change mitigation initiatives with all seriousness and work with the global community and institutions in this regard.&lt;/p&gt;
+&lt;p&gt;We will:&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Encourage Cleaner production.&lt;/li&gt;
+&lt;li&gt;Cleaner fuels will be promoted so as to bring down the pollution levels particularly in the cities.&lt;/li&gt;
+&lt;li&gt; The concept of pro-active 'Carbon Credit' will be promoted.&lt;/li&gt;
+&lt;li&gt; Ecological Audit of projects and pollution indexing of cities and townships will be done on scientific basis.&lt;/li&gt;
+&lt;li&gt; Pollution control mechanisms will be set up on priority basis.&lt;/li&gt;
+&lt;li&gt; In addition to protecting the existing forests and wildlife reserves, the wastelands of the country
+will be used for social forestry.&lt;/li&gt;
+&lt;li&gt; Guidelines for Green buildings and energy efficient work places will be brought out.&lt;/li&gt;
+&lt;li&gt; R&amp;amp;D and Human Resource Development in Environment Technology will be promoted.&lt;/li&gt;
+&lt;li&gt; Set up fool proof mechanisms for protection and preservation of wild life.&lt;/li&gt;
+&lt;li&gt; Encourage citizen's participation in reforestation, agro-forestry and social forestry, through targeted programmes.&lt;/li&gt;
+&lt;li&gt; Encourage and incentivize innovative garbage disposal and waste management practices, especially recycling techniques.
+&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>TheHimalayas</t>
   </si>
   <si>
@@ -964,6 +1498,17 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP is committed to serious endeavors for creating a global awareness regarding the conservation of Himalayas and will take the following steps:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Launch 'National Mission on Himalayas' as a unique programme of inter-governmental partnership, in coordinated policy making and capacity building across states and sectors.&lt;/li&gt;
+&lt;li&gt; Create a 'Himalayan Sustainability Fund'.&lt;/li&gt;
+&lt;li&gt; Create a Central University dedicated to the Himalayan Technology.&lt;/li&gt;
+&lt;li&gt; Give due Importance to the programmes devised to arrest the melting of Himalayan glaciers from which most of the rivers in North India originate.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>Natural&amp;NationalResourcesUseWhenRequiredProtectWhereNecessary</t>
   </si>
   <si>
@@ -973,6 +1518,20 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Indian belief has been best encapsulated in Gandhiji's words that "there is enough for everyone's need - but not for everyone's greed". Need is not the issue. Greed is. A country's progress depends upon its resources and how they are harnessed and protected. Those in power have to realize they are just trustees of the resources of the nation. The resources are neither meant for them nor for their masters. If we bring this basic shift in thinking of the Government, which Mahatma Gandhi also advocated, all problems will be resolved.&lt;/p&gt;
+&lt;p&gt;In recent years, it has been noticed that country's tangible and intangible resources have been looted with impunity. The adverse result is being felt on two sides: Firstly, the proceeds of the resources have not gone to the public exchequer. Secondly, because of this culture of usurping, the same resources are not available for public purposes. The management of natural resources is marred with either misappropriation or misallocation. This has to be set right.
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; We will set in place national policies on critical natural resources like coal, minerals, spectrum, etc. - spelling out in black and white how much should be utilized at what time and pace; how this should be strategically phased out to ensure sustainability; who should be allotted what responsibility of extraction and at what cost.&lt;/li&gt;
+&lt;li&gt; State Governments will be taken into confidence for harnessing of these resources.&lt;/li&gt;
+ &lt;li&gt;We will implement auction of precious resources through efficient mechanisms including e-
+ auction.&lt;/li&gt;
+&lt;li&gt; Resource mapping, exploration and management will be undertaken through the use of technology.&lt;/li&gt;
+&lt;li&gt; Value addition will be encouraged in all resources, instead of just marketing.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>SecureIndiansZeroToleranceonTerrorismExtremismandCrime</t>
   </si>
   <si>
@@ -982,6 +1541,14 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Comprehensive national security is not just about borders, but in its broad terms includes military security; economic security; cyber security; energy, food and water and health security; and social cohesion and harmony. To effectively address the issues of national security, we need to address the issues of - human resources, science and technology, system of governance and money.&lt;/p&gt;
+&lt;p&gt;National security cannot be compartmentalized based on one of issues but needs a clear roadmap to address it. Over the past decade, lack of a strong and visionary leadership, coupled with multiple power centres, has failed to address the issue of national security, leading to a chaotic situation and denting India's image in the international arena.&lt;/p&gt;
+&lt;p&gt;India has a sensitive neighbourhood and there are internal security issues. There have been intrusions inside the LAC (Line of actual control), loss of squadrons of combat aircraft by the air force, witnessing of a series of accidents by the Navy, leading to a loss in its combating capability built over many decades, communal riots, Maoist attacks, increase in incidence of Pakistan backed terror groups in India, illegal immigration across the eastern border, and racists' attacks in the national capital. All these are indications of surrendering of India's interest. This calls for a review and overhauling of the current system. With the financial situation worsening, the issue of national security can acquire a horrifying dimension.&lt;/p&gt;
+&lt;p&gt;BJP recognizes the importance of identifying a clear roadmap to address the issue head-on, with radical systemic changes.&lt;/p&gt;
+</t>
+  </si>
+  <si>
     <t>InternalSecurity</t>
   </si>
   <si>
@@ -991,6 +1558,22 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Revive the anti-terror mechanism that has been dismantled by the Congress, strengthen the role
+of NIA and put a system in place for swift and fair trial of terror related cases.&lt;/li&gt;
+&lt;li&gt; Reform the National Security Council to make it the hub of all sector-related assessments. It will be accountable for real-time intelligence dissemination. Digital and Cyber security will be a thrust area.&lt;/li&gt;
+&lt;li&gt; Insulate intelligence agencies from political intervention and interference.&lt;/li&gt;
+&lt;li&gt; Completely revamp the intelligence gathering system by modernizing the intelligence department.&lt;/li&gt;
+&lt;li&gt; Provide the State governments with all assistance to modernize their respective police forces and equip them with the latest technology. This will be taken up on a mission mode approach.&lt;/li&gt;
+&lt;li&gt; Strengthen and expand the Civil Defence and Home Guards mechanism to create a group of citizens for community defence, self-defence and disaster management.&lt;/li&gt;
+&lt;li&gt; Encourage and strengthen NCC training at the college and University level.&lt;/li&gt;
+&lt;li&gt; Chalk a national plan in consultation and participation of the state Governments, to address the challenges posed by the Maoist's insurgency. Talks with the insurgent groups will be conditional and within the framework of the constitution.&lt;/li&gt;
+&lt;li&gt; Take urgent steps for the safety of the migrant workers and communities from the Northeast and other states.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>ExternalSecurityItsBoundaryBeautyandBounty</t>
   </si>
   <si>
@@ -1000,6 +1583,29 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Address the issue of reforms with regards to defence equipment, support services, organizational
+reforms and other related matters.&lt;/li&gt;
+&lt;li&gt; Address the increasing shortage of commissioned and non-commissioned staff in the defence forces on a priority basis, in a time bound manner.&lt;/li&gt;
+&lt;li&gt; Implement one rank, one pension.&lt;/li&gt;
+&lt;li&gt; Build a War Memorial to recognize and honour the gallantry of our soldiers.&lt;/li&gt;
+&lt;li&gt; Take measures to make Short Service Commission more attractive.&lt;/li&gt;
+&lt;li&gt; Set up the National Maritime Authority which will be equipped with the best of infrastructure, and will focus on coastal security.&lt;/li&gt;
+&lt;li&gt; Modernize armed forces, and increase the R&amp;amp;D in defence, with a goal of developing indigenous defence technologies and fast tracking of defence purchases.&lt;/li&gt;
+&lt;li&gt; Deal with cross border terrorism with a firm hand.&lt;/li&gt;
+&lt;li&gt; Review and improve the border management. Punitive measures will be introduced to check illegal immigration.&lt;/li&gt;
+&lt;li&gt; Set up four dedicated defence universities to meet the shortage of manpower.&lt;/li&gt;
+&lt;li&gt; Appoint a Veterans Commission to address the grievances of veterans, including reforming ECHS and re-employment of ex-servicemen.&lt;/li&gt;
+ &lt;li&gt;Ensure greater participation of Armed Forces in the decision-making process of the Ministry of Defence.&lt;/li&gt;
+&lt;li&gt; Implement measures to improve the efficiency of Armed Forces Tribunals, and minimize appeals by the Government.&lt;/li&gt;
+&lt;li&gt; Ensure that servicemen can register and vote from their place of posting.&lt;/li&gt;
+&lt;li&gt; Initiate the process of digitization of defence land in cantonment and in other places.&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+  </si>
+  <si>
     <t>DefenceProduction</t>
   </si>
   <si>
@@ -1009,6 +1615,17 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;With its skilled human resources and technical talent, India can emerge as a global platform for defence hardware manufacture and software production. BJP will strengthen the Defence Research and Development Organization (DRDO); encourage private sector participation and investment, including
+FDI in selected defence industries.
+&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Technology transfer in defence manufacturing will be encouraged to the maximum.&lt;/li&gt;
+&lt;li&gt; We will find solutions to the problems hampering the growth of the defence sector.&lt;/li&gt;
+&lt;li&gt; We will encourage domestic industry to have a larger share in design and production of military hardware and platforms for both domestic use and exports, in a competitive environment.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>IndependentStrategicNuclearProgramme</t>
   </si>
   <si>
@@ -1018,6 +1635,17 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;
+BJP believes that the strategic gains acquired by India during the Atal Bihari Vajpayee regime on the nuclear programme have been frittered away by the Congress. Our emphasis was, and remains on, beginning of a new thrust on framing policies that would serve India's national interest in the 21st century. We will follow a two-pronged independent nuclear programme, unencumbered by foreign pressure and influence, for civilian and military purposes, especially as nuclear power is a major contributor to India's energy sector.&lt;/p&gt;
+&lt;p&gt;BJP will:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Study in detail India's nuclear doctrine, and revise and update it, to make it relevant to challenges of current times.&lt;/li&gt;
+&lt;li&gt; Maintain a credible minimum deterrent that is in tune with changing geostatic realities.&lt;/li&gt;
+&lt;li&gt; Invest in India's indigenous Thorium Technology Programme.&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>ForeignRelationsNationFirstUniversalBrotherhood</t>
   </si>
   <si>
@@ -1027,6 +1655,27 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>&lt;p&gt;BJP believes a resurgent India must get its rightful place in the comity of nations and international institutions. The vision is to fundamentally reboot and reorient the foreign policy goals, content and process, in a manner that locates India's global strategic engagement in a new paradigm and on a wider canvass, that is not just limited to political diplomacy, but also includes our economic, scientific, cultural, political and security interests, both regional and global, on the principles of equality and mutuality, so that it leads to an economically stronger India, and its voice is heard in the international fora.&lt;/p&gt;
+&lt;p&gt;BJP believes that political stability, progress and peace in the region are essential for south Asia's growth and development. The Congress-led UPA has failed to establish enduring friendly and cooperative relations with India's neighbours. India's relations with traditional allies have turned cold. India and its neighbours have drifted apart. Instead of clarity, we have seen confusion. The absence of statecraft has never been felt so acutely as today. India is seen to be floundering, whereas it should have been engaging with the world with confidence. The collapse of the Indian economy has contributed to the sorry state of foreign affairs in no small measure.&lt;/p&gt;
+&lt;p&gt;We will build a strong, self-reliant and self-confident India, regaining its rightful place in the comity of nations. In this, we will be firstly guided by our centuries old tradition of olq/kSo dqVqEcde~. At the same
+time, our foreign policy will be based on best National interests. We will create a web of allies to mutually further our interests. We will leverage all our resources and people to play a greater role on the international high table.&lt;/p&gt;
+&lt;p&gt;India has long failed to duly appreciate the full extent and gamut of its soft power potential. There is a need to integrate our soft power avenues into our external interchange, particularly, harnessing and focusing on the spiritual, cultural and philosophical dimensions of it. India has always played a major role in world affairs, offering a lot to the World. This has been its tradition since time immemorial. The magnetic power of India has always been in its ancient wisdom and heritage, elucidating principles like harmony and equity. This continues to be equally relevant to the world today in today's times of Soft power. We will adopt Proactive Diplomacy to spread the same. India was reckoned not only as Vishwaguru but also a vibrant trading society. Our ancestors used to trade with foreign nations through the routes of sea, centuries ago. This was based on the strength of our business acumen and integrity, our products and crafts. The symbols of our ancient civilizations stand as a testimony to our architectural and urban planning excellence. We will revive Brand India with the help of our strengths of 5 T's: Tradition, Talent, Tourism, Trade and Technology.&lt;/p&gt;
+&lt;p&gt;Guiding Principles of our Foreign Policy will be:&lt;/p&gt;
+&lt;ul&gt;
+&lt;li&gt; Equations will be mended through pragmatism and a doctrine of mutually beneficial and interlocking relationships, based on enlightened national interest.&lt;/li&gt;
+&lt;li&gt; We will champion uniform international opinion on issues like Terrorism and Global Warming.&lt;/li&gt;
+&lt;li&gt; Instead of being led by big power interests, we will engage proactively on our own with countries in
+the neighbourhood and beyond.&lt;/li&gt;
+&lt;li&gt; In our neighbourhood we will pursue friendly relations. However, where required we will not hesitate from taking strong stand and steps.&lt;/li&gt;
+&lt;li&gt; We will work towards strengthening Regional forums like SAARC and ASEAN.&lt;/li&gt;
+&lt;li&gt; We will continue our dialogue, engagement and cooperation, with global forums like BRICS, G20. IBSA, SCO and ASEM. States will be encouraged to play a greater role in diplomacy; actively building relations with foreign countries to harness their mutual cultural and commercial strengths.&lt;/li&gt;
+&lt;li&gt; We will expand and empower our pool of diplomats, ensuring our message is taken to the world and our great nation represented on the whole in a befitting manner.&lt;/li&gt;
+&lt;li&gt; The NRIs, PIOs and professionals settled abroad are a vast reservoir to articulate the national interests and affairs globally. This resource will be harnessed for strengthening Brand India.&lt;/li&gt;
+&lt;li&gt; India shall remain a natural home for persecuted Hindus and they shall be welcome to seek refuge here.
+&lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>CulturalHeritage</t>
   </si>
   <si>
@@ -1036,6 +1685,22 @@
     <t>Leap Forward</t>
   </si>
   <si>
+    <t>
+&lt;p&gt;Ram Mandir: BJP reiterates its stand to explore all possibilities within the framework of the constitution to facilitate the construction of the Ram Temple in Ayodhya.&lt;/p&gt;
+&lt;p&gt;Ram Setu: Ram Setu is a part of our cultural heritage and also of strategic importance due to its vast thorium deposits. These facts will be taken into consideration while taking any decision on 'Sethu- Samudram Channel' project.&lt;/p&gt;
+&lt;p&gt;Ganga: River Ganga is a symbol of faith in India, and has a special place in the Indian psyche. It is Mukti dayini. In addition it is also Jivan dayini for the parts of the country it flows. People and cattle depend on it for agriculture, fodder and drinking water. Pure water of the Ganga are thus essential for the spiritual as well as physical well being of India.&lt;/p&gt;
+&lt;p&gt;Unfortunately however, even after decades of independence, the Ganga continues to be polluted and is drying. BJP commits to ensure the cleanliness, purity and uninterrupted flow of the Ganga on priority. In addition, a massive 'Clean Rivers Programme' will be launched across the country driven by people's participation.&lt;/p&gt;
+&lt;p&gt;Cow and its Progeny: In view of the contribution of cow and its progeny to agriculture, socio-economic and cultural life of our country, the Department of Animal Husbandry will be suitably strengthened and empowered for the protection and promotion of cow and its progeny.&lt;/p&gt;
+&lt;ul&gt;
+ &lt;li&gt;Necessary legal framework will be created to protect and promote cow and its progeny.&lt;/li&gt;
+ &lt;li&gt;A National Cattle Development board will be set up to implement a Programme for the improvement of indigenous livestock breeds.&lt;/li&gt;
+&lt;/ul&gt;
+&lt;p&gt;Heritage Sites: We will provide appropriate resources for the maintenance and restoration of all national heritage sites, and to prevent their vandalisation in any form. The digitization of archives and archeological and museological records would be initiated. A National Mission for beautifying and improving the infrastructure and amenities at pilgrimage centres of all faiths will be launched.&lt;/p&gt;
+&lt;p&gt;Languages: Indian Languages are repositories of our rich literature, history, culture, art and scientific achievements. Many of our dialects are important source for knowing our heritage. BJP would promote Indian languages, and put measures for the development of all Indian languages, so that they become a powerful vehicle for creating a knowledge society.
+&lt;/p&gt;
+</t>
+  </si>
+  <si>
     <t>UniformCivilCode</t>
   </si>
   <si>
@@ -1043,6 +1708,9 @@
   </si>
   <si>
     <t>Leap Forward</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Article 44 of the constitution of India lists Uniform Civil Code as one of the Directive Principles of state policy. BJP believes that there cannot be gender equality till such time India adopts a Uniform Civil Code, which protects the rights of all women, and the BJP reiterates its stand to draft a Uniform Civil Code, drawing upon the best traditions and harmonizing them with the modern times.&lt;/p&gt;</t>
   </si>
 </sst>
 </file>
@@ -1509,511 +2177,649 @@
       <c t="s" s="1" r="C29">
         <v>111</v>
       </c>
+      <c t="s" s="1" r="D29">
+        <v>112</v>
+      </c>
     </row>
     <row r="30">
       <c t="s" s="1" r="A30">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c t="s" s="1" r="B30">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c t="s" s="1" r="C30">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c t="s" s="1" r="D30">
+        <v>116</v>
       </c>
     </row>
     <row r="31">
       <c t="s" s="1" r="A31">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c t="s" s="1" r="B31">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c t="s" s="1" r="C31">
-        <v>117</v>
+        <v>119</v>
+      </c>
+      <c t="s" s="1" r="D31">
+        <v>120</v>
       </c>
     </row>
     <row r="32">
       <c t="s" s="1" r="A32">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c t="s" s="1" r="B32">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c t="s" s="1" r="C32">
-        <v>120</v>
+        <v>123</v>
+      </c>
+      <c t="s" s="1" r="D32">
+        <v>124</v>
       </c>
     </row>
     <row r="33">
       <c t="s" s="1" r="A33">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c t="s" s="1" r="B33">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c t="s" s="1" r="C33">
-        <v>123</v>
+        <v>127</v>
+      </c>
+      <c t="s" s="1" r="D33">
+        <v>128</v>
       </c>
     </row>
     <row r="34">
       <c t="s" s="1" r="A34">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c t="s" s="1" r="B34">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c t="s" s="1" r="C34">
-        <v>126</v>
+        <v>131</v>
+      </c>
+      <c t="s" s="1" r="D34">
+        <v>132</v>
       </c>
     </row>
     <row r="35">
       <c t="s" s="1" r="A35">
-        <v>127</v>
+        <v>133</v>
       </c>
       <c t="s" s="1" r="B35">
-        <v>128</v>
+        <v>134</v>
       </c>
       <c t="s" s="1" r="C35">
-        <v>129</v>
+        <v>135</v>
+      </c>
+      <c t="s" s="1" r="D35">
+        <v>136</v>
       </c>
     </row>
     <row r="36">
       <c t="s" s="1" r="A36">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c t="s" s="1" r="B36">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c t="s" s="1" r="C36">
-        <v>132</v>
+        <v>139</v>
+      </c>
+      <c t="s" s="1" r="D36">
+        <v>140</v>
       </c>
     </row>
     <row r="37">
       <c t="s" s="1" r="A37">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c t="s" s="1" r="B37">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c t="s" s="1" r="C37">
-        <v>135</v>
+        <v>143</v>
+      </c>
+      <c t="s" s="1" r="D37">
+        <v>144</v>
       </c>
     </row>
     <row r="38">
       <c t="s" s="1" r="A38">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c t="s" s="1" r="B38">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c t="s" s="1" r="C38">
-        <v>138</v>
+        <v>147</v>
+      </c>
+      <c t="s" s="1" r="D38">
+        <v>148</v>
       </c>
     </row>
     <row r="39">
       <c t="s" s="1" r="A39">
-        <v>139</v>
+        <v>149</v>
       </c>
       <c t="s" s="1" r="B39">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c t="s" s="1" r="C39">
-        <v>141</v>
+        <v>151</v>
+      </c>
+      <c t="s" s="1" r="D39">
+        <v>152</v>
       </c>
     </row>
     <row r="40">
       <c t="s" s="1" r="A40">
-        <v>142</v>
+        <v>153</v>
       </c>
       <c t="s" s="1" r="B40">
-        <v>143</v>
+        <v>154</v>
       </c>
       <c t="s" s="1" r="C40">
-        <v>144</v>
+        <v>155</v>
+      </c>
+      <c t="s" s="1" r="D40">
+        <v>156</v>
       </c>
     </row>
     <row r="41">
       <c t="s" s="1" r="A41">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c t="s" s="1" r="B41">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c t="s" s="1" r="C41">
-        <v>147</v>
+        <v>159</v>
+      </c>
+      <c t="s" s="1" r="D41">
+        <v>160</v>
       </c>
     </row>
     <row r="42">
       <c t="s" s="1" r="A42">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c t="s" s="1" r="B42">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c t="s" s="1" r="C42">
-        <v>150</v>
+        <v>163</v>
+      </c>
+      <c t="s" s="1" r="D42">
+        <v>164</v>
       </c>
     </row>
     <row r="43">
       <c t="s" s="1" r="A43">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c t="s" s="1" r="B43">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c t="s" s="1" r="C43">
-        <v>153</v>
+        <v>167</v>
+      </c>
+      <c t="s" s="1" r="D43">
+        <v>168</v>
       </c>
     </row>
     <row r="44">
       <c t="s" s="1" r="A44">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c t="s" s="1" r="B44">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c t="s" s="1" r="C44">
-        <v>156</v>
+        <v>171</v>
+      </c>
+      <c t="s" s="1" r="D44">
+        <v>172</v>
       </c>
     </row>
     <row r="45">
       <c t="s" s="1" r="A45">
-        <v>157</v>
+        <v>173</v>
       </c>
       <c t="s" s="1" r="B45">
-        <v>158</v>
+        <v>174</v>
       </c>
       <c t="s" s="1" r="C45">
-        <v>159</v>
+        <v>175</v>
+      </c>
+      <c t="s" s="1" r="D45">
+        <v>176</v>
       </c>
     </row>
     <row r="46">
       <c t="s" s="1" r="A46">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c t="s" s="1" r="B46">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c t="s" s="1" r="C46">
-        <v>162</v>
+        <v>179</v>
+      </c>
+      <c t="s" s="1" r="D46">
+        <v>180</v>
       </c>
     </row>
     <row r="47">
       <c t="s" s="1" r="A47">
-        <v>163</v>
+        <v>181</v>
       </c>
       <c t="s" s="1" r="B47">
-        <v>164</v>
+        <v>182</v>
       </c>
       <c t="s" s="1" r="C47">
-        <v>165</v>
+        <v>183</v>
+      </c>
+      <c t="s" s="1" r="D47">
+        <v>184</v>
       </c>
     </row>
     <row r="48">
       <c t="s" s="1" r="A48">
-        <v>166</v>
+        <v>185</v>
       </c>
       <c t="s" s="1" r="B48">
-        <v>167</v>
+        <v>186</v>
       </c>
       <c t="s" s="1" r="C48">
-        <v>168</v>
+        <v>187</v>
+      </c>
+      <c t="s" s="1" r="D48">
+        <v>188</v>
       </c>
     </row>
     <row r="49">
       <c t="s" s="1" r="A49">
-        <v>169</v>
+        <v>189</v>
       </c>
       <c t="s" s="1" r="B49">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c t="s" s="1" r="C49">
-        <v>171</v>
+        <v>191</v>
+      </c>
+      <c t="s" s="1" r="D49">
+        <v>192</v>
       </c>
     </row>
     <row r="50">
       <c t="s" s="1" r="A50">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c t="s" s="1" r="B50">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c t="s" s="1" r="C50">
-        <v>174</v>
+        <v>195</v>
+      </c>
+      <c t="s" s="1" r="D50">
+        <v>196</v>
       </c>
     </row>
     <row r="51">
       <c t="s" s="1" r="A51">
-        <v>175</v>
+        <v>197</v>
       </c>
       <c t="s" s="1" r="B51">
-        <v>176</v>
+        <v>198</v>
       </c>
       <c t="s" s="1" r="C51">
-        <v>177</v>
+        <v>199</v>
+      </c>
+      <c t="s" s="1" r="D51">
+        <v>200</v>
       </c>
     </row>
     <row r="52">
       <c t="s" s="1" r="A52">
-        <v>178</v>
+        <v>201</v>
       </c>
       <c t="s" s="1" r="B52">
-        <v>179</v>
+        <v>202</v>
       </c>
       <c t="s" s="1" r="C52">
-        <v>180</v>
+        <v>203</v>
+      </c>
+      <c t="s" s="1" r="D52">
+        <v>204</v>
       </c>
     </row>
     <row r="53">
       <c t="s" s="1" r="A53">
-        <v>181</v>
+        <v>205</v>
       </c>
       <c t="s" s="1" r="B53">
-        <v>182</v>
+        <v>206</v>
       </c>
       <c t="s" s="1" r="C53">
-        <v>183</v>
+        <v>207</v>
       </c>
     </row>
     <row r="54">
       <c t="s" s="1" r="A54">
-        <v>184</v>
+        <v>208</v>
       </c>
       <c t="s" s="1" r="B54">
-        <v>185</v>
+        <v>209</v>
       </c>
       <c t="s" s="1" r="C54">
-        <v>186</v>
+        <v>210</v>
+      </c>
+      <c t="s" s="1" r="D54">
+        <v>211</v>
       </c>
     </row>
     <row r="55">
       <c t="s" s="1" r="A55">
-        <v>187</v>
+        <v>212</v>
       </c>
       <c t="s" s="1" r="B55">
-        <v>188</v>
+        <v>213</v>
       </c>
       <c t="s" s="1" r="C55">
-        <v>189</v>
+        <v>214</v>
+      </c>
+      <c t="s" s="1" r="D55">
+        <v>215</v>
       </c>
     </row>
     <row r="56">
       <c t="s" s="1" r="A56">
-        <v>190</v>
+        <v>216</v>
       </c>
       <c t="s" s="1" r="B56">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c t="s" s="1" r="C56">
-        <v>192</v>
+        <v>218</v>
+      </c>
+      <c t="s" s="1" r="D56">
+        <v>219</v>
       </c>
     </row>
     <row r="57">
       <c t="s" s="1" r="A57">
-        <v>193</v>
+        <v>220</v>
       </c>
       <c t="s" s="1" r="B57">
-        <v>194</v>
+        <v>221</v>
       </c>
       <c t="s" s="1" r="C57">
-        <v>195</v>
+        <v>222</v>
+      </c>
+      <c t="s" s="1" r="D57">
+        <v>223</v>
       </c>
     </row>
     <row r="58">
       <c t="s" s="1" r="A58">
-        <v>196</v>
+        <v>224</v>
       </c>
       <c t="s" s="1" r="B58">
-        <v>197</v>
+        <v>225</v>
       </c>
       <c t="s" s="1" r="C58">
-        <v>198</v>
+        <v>226</v>
+      </c>
+      <c t="s" s="1" r="D58">
+        <v>227</v>
       </c>
     </row>
     <row r="59">
       <c t="s" s="1" r="A59">
-        <v>199</v>
+        <v>228</v>
       </c>
       <c t="s" s="1" r="B59">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c t="s" s="1" r="C59">
-        <v>201</v>
+        <v>230</v>
+      </c>
+      <c t="s" s="1" r="D59">
+        <v>231</v>
       </c>
     </row>
     <row r="60">
       <c t="s" s="1" r="A60">
-        <v>202</v>
+        <v>232</v>
       </c>
       <c t="s" s="1" r="B60">
-        <v>203</v>
+        <v>233</v>
       </c>
       <c t="s" s="1" r="C60">
-        <v>204</v>
+        <v>234</v>
+      </c>
+      <c t="s" s="1" r="D60">
+        <v>235</v>
       </c>
     </row>
     <row r="61">
       <c t="s" s="1" r="A61">
-        <v>205</v>
+        <v>236</v>
       </c>
       <c t="s" s="1" r="B61">
-        <v>206</v>
+        <v>237</v>
       </c>
       <c t="s" s="1" r="C61">
-        <v>207</v>
+        <v>238</v>
+      </c>
+      <c t="s" s="1" r="D61">
+        <v>239</v>
       </c>
     </row>
     <row r="62">
       <c t="s" s="1" r="A62">
-        <v>208</v>
+        <v>240</v>
       </c>
       <c t="s" s="1" r="B62">
-        <v>209</v>
+        <v>241</v>
       </c>
       <c t="s" s="1" r="C62">
-        <v>210</v>
+        <v>242</v>
+      </c>
+      <c t="s" s="1" r="D62">
+        <v>243</v>
       </c>
     </row>
     <row r="63">
       <c t="s" s="1" r="A63">
-        <v>211</v>
+        <v>244</v>
       </c>
       <c t="s" s="1" r="B63">
-        <v>212</v>
+        <v>245</v>
       </c>
       <c t="s" s="1" r="C63">
-        <v>213</v>
+        <v>246</v>
+      </c>
+      <c t="s" s="1" r="D63">
+        <v>247</v>
       </c>
     </row>
     <row r="64">
       <c t="s" s="1" r="A64">
-        <v>214</v>
+        <v>248</v>
       </c>
       <c t="s" s="1" r="B64">
-        <v>215</v>
+        <v>249</v>
       </c>
       <c t="s" s="1" r="C64">
-        <v>216</v>
+        <v>250</v>
+      </c>
+      <c t="s" s="1" r="D64">
+        <v>251</v>
       </c>
     </row>
     <row r="65">
       <c t="s" s="1" r="A65">
-        <v>217</v>
+        <v>252</v>
       </c>
       <c t="s" s="1" r="B65">
-        <v>218</v>
+        <v>253</v>
       </c>
       <c t="s" s="1" r="C65">
-        <v>219</v>
+        <v>254</v>
+      </c>
+      <c t="s" s="1" r="D65">
+        <v>255</v>
       </c>
     </row>
     <row r="66">
       <c t="s" s="1" r="A66">
-        <v>220</v>
+        <v>256</v>
       </c>
       <c t="s" s="1" r="B66">
-        <v>221</v>
+        <v>257</v>
       </c>
       <c t="s" s="1" r="C66">
-        <v>222</v>
+        <v>258</v>
+      </c>
+      <c t="s" s="1" r="D66">
+        <v>259</v>
       </c>
     </row>
     <row r="67">
       <c t="s" s="1" r="A67">
-        <v>223</v>
+        <v>260</v>
       </c>
       <c t="s" s="1" r="B67">
-        <v>224</v>
+        <v>261</v>
       </c>
       <c t="s" s="1" r="C67">
-        <v>225</v>
+        <v>262</v>
+      </c>
+      <c t="s" s="1" r="D67">
+        <v>263</v>
       </c>
     </row>
     <row r="68">
       <c t="s" s="1" r="A68">
-        <v>226</v>
+        <v>264</v>
       </c>
       <c t="s" s="1" r="B68">
-        <v>227</v>
+        <v>265</v>
       </c>
       <c t="s" s="1" r="C68">
-        <v>228</v>
+        <v>266</v>
+      </c>
+      <c t="s" s="1" r="D68">
+        <v>267</v>
       </c>
     </row>
     <row r="69">
       <c t="s" s="1" r="A69">
-        <v>229</v>
+        <v>268</v>
       </c>
       <c t="s" s="1" r="B69">
-        <v>230</v>
+        <v>269</v>
       </c>
       <c t="s" s="1" r="C69">
-        <v>231</v>
+        <v>270</v>
+      </c>
+      <c t="s" s="1" r="D69">
+        <v>271</v>
       </c>
     </row>
     <row r="70">
       <c t="s" s="1" r="A70">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c t="s" s="1" r="B70">
-        <v>233</v>
+        <v>273</v>
       </c>
       <c t="s" s="1" r="C70">
-        <v>234</v>
+        <v>274</v>
+      </c>
+      <c t="s" s="1" r="D70">
+        <v>275</v>
       </c>
     </row>
     <row r="71">
       <c t="s" s="1" r="A71">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c t="s" s="1" r="B71">
-        <v>236</v>
+        <v>277</v>
       </c>
       <c t="s" s="1" r="C71">
-        <v>237</v>
+        <v>278</v>
+      </c>
+      <c t="s" s="1" r="D71">
+        <v>279</v>
       </c>
     </row>
     <row r="72">
       <c t="s" s="1" r="A72">
-        <v>238</v>
+        <v>280</v>
       </c>
       <c t="s" s="1" r="B72">
-        <v>239</v>
+        <v>281</v>
       </c>
       <c t="s" s="1" r="C72">
-        <v>240</v>
+        <v>282</v>
+      </c>
+      <c t="s" s="1" r="D72">
+        <v>283</v>
       </c>
     </row>
     <row r="73">
       <c t="s" s="1" r="A73">
-        <v>241</v>
+        <v>284</v>
       </c>
       <c t="s" s="1" r="B73">
-        <v>242</v>
+        <v>285</v>
       </c>
       <c t="s" s="1" r="C73">
-        <v>243</v>
+        <v>286</v>
+      </c>
+      <c t="s" s="1" r="D73">
+        <v>287</v>
       </c>
     </row>
     <row r="74">
       <c t="s" s="1" r="A74">
-        <v>244</v>
+        <v>288</v>
       </c>
       <c t="s" s="1" r="B74">
-        <v>245</v>
+        <v>289</v>
       </c>
       <c t="s" s="1" r="C74">
-        <v>246</v>
+        <v>290</v>
+      </c>
+      <c t="s" s="1" r="D74">
+        <v>291</v>
       </c>
     </row>
     <row r="75">
       <c t="s" s="1" r="A75">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c t="s" s="1" r="B75">
-        <v>248</v>
+        <v>293</v>
       </c>
       <c t="s" s="1" r="C75">
-        <v>249</v>
+        <v>294</v>
+      </c>
+      <c t="s" s="1" r="D75">
+        <v>295</v>
       </c>
     </row>
   </sheetData>

</xml_diff>